<commit_message>
added separate course prices
</commit_message>
<xml_diff>
--- a/розрахунок вартості шаблон бакалавр 2 рік.xlsx
+++ b/розрахунок вартості шаблон бакалавр 2 рік.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учеба\8_семестр\диплом\term_paper_3d_grade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5509B0A0-6FDB-415D-9F9C-34BE6802AEB1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E79E59-45FE-46C5-B09E-FD688C3F0026}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2295,7 +2295,7 @@
   <dimension ref="A2:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,7 +2563,7 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,11 +2639,11 @@
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2676,11 +2676,11 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2713,11 +2713,11 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2750,11 +2750,11 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2787,11 +2787,11 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2824,11 +2824,11 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2861,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2898,11 +2898,11 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2935,11 +2935,11 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -2972,11 +2972,11 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I12" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3009,11 +3009,11 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I13" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3046,11 +3046,11 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3083,11 +3083,11 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3120,11 +3120,11 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3157,11 +3157,11 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I17" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3194,11 +3194,11 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I18" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3231,11 +3231,11 @@
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I19" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3268,11 +3268,11 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I20" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3305,11 +3305,11 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I21" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3342,11 +3342,11 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3379,11 +3379,11 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I23" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3416,11 +3416,11 @@
         <v>0</v>
       </c>
       <c r="H24" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I24" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3453,11 +3453,11 @@
         <v>0</v>
       </c>
       <c r="H25" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I25" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3490,11 +3490,11 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I26" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3527,11 +3527,11 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I27" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3564,11 +3564,11 @@
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I28" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3601,11 +3601,11 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I29" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3638,11 +3638,11 @@
         <v>0</v>
       </c>
       <c r="H30" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I30" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3675,11 +3675,11 @@
         <v>0</v>
       </c>
       <c r="H31" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I31" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3712,11 +3712,11 @@
         <v>0</v>
       </c>
       <c r="H32" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I32" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3749,11 +3749,11 @@
         <v>0</v>
       </c>
       <c r="H33" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I33" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3786,11 +3786,11 @@
         <v>0</v>
       </c>
       <c r="H34" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I34" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3823,11 +3823,11 @@
         <v>0</v>
       </c>
       <c r="H35" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I35" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3860,11 +3860,11 @@
         <v>0</v>
       </c>
       <c r="H36" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I36" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3897,11 +3897,11 @@
         <v>0</v>
       </c>
       <c r="H37" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I37" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3934,11 +3934,11 @@
         <v>0</v>
       </c>
       <c r="H38" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I38" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3971,11 +3971,11 @@
         <v>0</v>
       </c>
       <c r="H39" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I39" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4008,11 +4008,11 @@
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I40" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4045,11 +4045,11 @@
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I41" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4082,11 +4082,11 @@
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I42" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4119,11 +4119,11 @@
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I43" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4156,11 +4156,11 @@
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I44" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4193,11 +4193,11 @@
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I45" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4230,11 +4230,11 @@
         <v>0</v>
       </c>
       <c r="H46" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I46" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4267,11 +4267,11 @@
         <v>0</v>
       </c>
       <c r="H47" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I47" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4304,11 +4304,11 @@
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I48" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4341,11 +4341,11 @@
         <v>0</v>
       </c>
       <c r="H49" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I49" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4378,11 +4378,11 @@
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I50" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4415,11 +4415,11 @@
         <v>0</v>
       </c>
       <c r="H51" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I51" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4452,11 +4452,11 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I52" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4489,11 +4489,11 @@
         <v>0</v>
       </c>
       <c r="H53" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I53" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4526,11 +4526,11 @@
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I54" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4563,11 +4563,11 @@
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I55" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4600,11 +4600,11 @@
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I56" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4637,11 +4637,11 @@
         <v>0</v>
       </c>
       <c r="H57" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I57" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4674,11 +4674,11 @@
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I58" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4711,11 +4711,11 @@
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I59" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4748,11 +4748,11 @@
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I60" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4785,11 +4785,11 @@
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I61" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4822,11 +4822,11 @@
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I62" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4859,11 +4859,11 @@
         <v>0</v>
       </c>
       <c r="H63" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I63" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4896,11 +4896,11 @@
         <v>0</v>
       </c>
       <c r="H64" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I64" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4933,11 +4933,11 @@
         <v>0</v>
       </c>
       <c r="H65" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I65" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4970,11 +4970,11 @@
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5007,11 +5007,11 @@
         <v>0</v>
       </c>
       <c r="H67" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I67" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5044,11 +5044,11 @@
         <v>0</v>
       </c>
       <c r="H68" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I68" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5081,11 +5081,11 @@
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I69" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5118,11 +5118,11 @@
         <v>0</v>
       </c>
       <c r="H70" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I70" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5155,11 +5155,11 @@
         <v>0</v>
       </c>
       <c r="H71" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I71" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5192,11 +5192,11 @@
         <v>0</v>
       </c>
       <c r="H72" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I72" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5229,11 +5229,11 @@
         <v>0</v>
       </c>
       <c r="H73" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I73" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5266,11 +5266,11 @@
         <v>0</v>
       </c>
       <c r="H74" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I74" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5303,11 +5303,11 @@
         <v>0</v>
       </c>
       <c r="H75" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I75" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5340,11 +5340,11 @@
         <v>0</v>
       </c>
       <c r="H76" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I76" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5377,11 +5377,11 @@
         <v>0</v>
       </c>
       <c r="H77" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I77" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5414,11 +5414,11 @@
         <v>0</v>
       </c>
       <c r="H78" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I78" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5451,11 +5451,11 @@
         <v>0</v>
       </c>
       <c r="H79" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I79" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5488,11 +5488,11 @@
         <v>0</v>
       </c>
       <c r="H80" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I80" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5525,11 +5525,11 @@
         <v>0</v>
       </c>
       <c r="H81" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I81" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5562,11 +5562,11 @@
         <v>0</v>
       </c>
       <c r="H82" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I82" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5599,11 +5599,11 @@
         <v>0</v>
       </c>
       <c r="H83" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I83" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5636,11 +5636,11 @@
         <v>0</v>
       </c>
       <c r="H84" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I84" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5673,11 +5673,11 @@
         <v>0</v>
       </c>
       <c r="H85" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I85" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5710,11 +5710,11 @@
         <v>0</v>
       </c>
       <c r="H86" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I86" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5747,11 +5747,11 @@
         <v>0</v>
       </c>
       <c r="H87" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I87" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5784,11 +5784,11 @@
         <v>0</v>
       </c>
       <c r="H88" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I88" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5821,11 +5821,11 @@
         <v>0</v>
       </c>
       <c r="H89" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I89" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5858,11 +5858,11 @@
         <v>0</v>
       </c>
       <c r="H90" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I90" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5895,11 +5895,11 @@
         <v>0</v>
       </c>
       <c r="H91" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I91" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5932,11 +5932,11 @@
         <v>0</v>
       </c>
       <c r="H92" s="1">
-        <f>'1-й курс'!$AB$2</f>
+        <f>('1-й курс'!$AB$2+'2-й курс'!$AB$2)/2</f>
         <v>0</v>
       </c>
       <c r="I92" s="1">
-        <f>'1-й курс'!$AC$2</f>
+        <f>('1-й курс'!$AC$2+'2-й курс'!$AC$2)/2</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>